<commit_message>
delete and reset functionality added
</commit_message>
<xml_diff>
--- a/bills.xlsx
+++ b/bills.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stran\IdeaProjects\verisoftBill\"/>
     </mc:Choice>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>[fanta - 5]</t>
   </si>
@@ -148,12 +148,40 @@
   </si>
   <si>
     <t>815.86</t>
+  </si>
+  <si>
+    <t>2019-11-12</t>
+  </si>
+  <si>
+    <t>sumant gupta</t>
+  </si>
+  <si>
+    <t>matihani</t>
+  </si>
+  <si>
+    <t>9824840876</t>
+  </si>
+  <si>
+    <t>[sugar - 1, suji - 20]</t>
+  </si>
+  <si>
+    <t>870</t>
+  </si>
+  <si>
+    <t>101.79</t>
+  </si>
+  <si>
+    <t>884.79</t>
+  </si>
+  <si>
+    <t>2019-11-14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -482,15 +510,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.6328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="70" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.36328125" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.6328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="70.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.1796875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="10.36328125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -716,6 +744,55 @@
         <v>42</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>47.499999999999886</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>